<commit_message>
Updated testbed parts list
</commit_message>
<xml_diff>
--- a/testbed/parts_list.xlsx
+++ b/testbed/parts_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,12 +15,67 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>PART NAME</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>COST/UNIT</t>
+  </si>
+  <si>
+    <t>Utilite Standard</t>
+  </si>
+  <si>
+    <t>TOTAL COST</t>
+  </si>
+  <si>
+    <t>http://www.compulab.co.il/utilite-computer/web/utilite-availability</t>
+  </si>
+  <si>
+    <t>PART NO.</t>
+  </si>
+  <si>
+    <t>HP 2920-24G Network Switch</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/HP-J9726A-2920-24G-Switch/dp/B00BJ42JYG/ref=sr_1_1?ie=UTF8&amp;qid=1422292309&amp;sr=8-1&amp;keywords=J9726A</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -34,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,18 +97,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -62,7 +221,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="373737"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -343,36 +502,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="123.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5">
+        <v>159</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2544</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>872.95</v>
+      </c>
+      <c r="E3" s="4">
+        <v>872.95</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed to 48 port switch with 32 BBB
</commit_message>
<xml_diff>
--- a/testbed/parts_list.xlsx
+++ b/testbed/parts_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>URL</t>
   </si>
@@ -30,51 +30,21 @@
     <t>COST/UNIT</t>
   </si>
   <si>
-    <t>Utilite Standard</t>
-  </si>
-  <si>
     <t>TOTAL COST</t>
   </si>
   <si>
-    <t>http://www.compulab.co.il/utilite-computer/web/utilite-availability</t>
-  </si>
-  <si>
     <t>PART NO.</t>
   </si>
   <si>
-    <t>HP 2920-24G Network Switch</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/HP-J9726A-2920-24G-Switch/dp/B00BJ42JYG/ref=sr_1_1?ie=UTF8&amp;qid=1422292309&amp;sr=8-1&amp;keywords=J9726A</t>
-  </si>
-  <si>
     <t>Kingston MicroSD cards</t>
   </si>
   <si>
     <t>http://www.amazon.com/Kingston-Digital-microSDHC-SDC4-16GBET/dp/B00DYQYLQQ/ref=sr_1_1?ie=UTF8&amp;qid=1422292553&amp;sr=8-1&amp;keywords=micro+sd+16gb</t>
   </si>
   <si>
-    <t>istarUSA WN228 server rack chassis</t>
-  </si>
-  <si>
-    <t>http://www.istarusa.com/istarusa/products.php?model=WN228</t>
-  </si>
-  <si>
-    <t>http://www.istarusa.com/istarusa/products.php?model=WA-PS010</t>
-  </si>
-  <si>
-    <t>http://www.tigerdirect.com/applications/SearchTools/item-details.asp?EdpNo=3301357</t>
-  </si>
-  <si>
     <t>Total Cost:</t>
   </si>
   <si>
-    <t>istarUSA WA-PS010 rack-mount power outlets</t>
-  </si>
-  <si>
-    <t>istarUSA WA-SF80B flat vented tray</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/Cable-Matters-5-Color-Snagless-Ethernet/dp/B00E5I7VJG/ref=sr_1_1?s=pc&amp;ie=UTF8&amp;qid=1422383476&amp;sr=1-1&amp;keywords=ethernet+cables</t>
   </si>
   <si>
@@ -85,6 +55,30 @@
   </si>
   <si>
     <t>TRENDnet 24-Port Unmanaged Gigabit switch</t>
+  </si>
+  <si>
+    <t>HP 2920-48G Network Switch</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/HP-J9728A-2920-48G-Switch/dp/B00BJ42JQY</t>
+  </si>
+  <si>
+    <t>BeagleBone Black</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/BeagleBoard-by-CircuitCo/BB-BBLK-000/?qs=%2fha2pyFadugh6wNMONnDuAbTwbrIHVw4R%2f%252bth5Q2M%2fX2Gs60muroNw%3d%3d</t>
+  </si>
+  <si>
+    <t>10/100 Ethernet Adapter (w/ linux)</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16812315001&amp;cm_re=usb_ethernet-_-12-315-001-_-Product</t>
+  </si>
+  <si>
+    <t>min cables required</t>
+  </si>
+  <si>
+    <t>cables ordered</t>
   </si>
 </sst>
 </file>
@@ -484,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +497,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -515,7 +509,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>0</v>
@@ -526,20 +520,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D2" s="5">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="E2" s="4">
         <f>D2*C2</f>
-        <v>2544</v>
+        <v>1760</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -547,7 +541,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -560,7 +554,7 @@
         <v>872.95</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -568,80 +562,61 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4">
         <v>8.9499999999999993</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>143.19999999999999</v>
+        <v>286.39999999999998</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>699.99</v>
-      </c>
       <c r="E5" s="4">
         <f>D5*C5</f>
-        <v>699.99</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
       <c r="E6" s="4">
         <f t="shared" ref="E6:E9" si="1">D6*C6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D7" s="4">
-        <v>66.489999999999995</v>
+        <v>11.99</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
-        <v>332.45</v>
+        <v>383.68</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,20 +624,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4">
         <v>13</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,7 +645,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -683,31 +658,44 @@
         <v>96.99</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="D10" s="9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4">
         <f>SUM(E2:E9)</f>
-        <v>4819.579999999999</v>
+        <v>3595.0199999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2">
+        <f>C2*2</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2">
+        <f>C8*5</f>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F9" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updaed parts list with power supply
</commit_message>
<xml_diff>
--- a/testbed/parts_list.xlsx
+++ b/testbed/parts_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>URL</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>NETGEAR 48-Port 10/100/1000Mbps</t>
+  </si>
+  <si>
+    <t>Power  Supply</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=9SIA5H62KH2141&amp;cm_re=300W_5V_power_supply-_-0R7-001B-00027-_-Product</t>
+  </si>
+  <si>
+    <t>Power Supply Search</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/ProductList.aspx?Submit=ENE&amp;DEPA=0&amp;Order=BESTMATCH&amp;Description=300W+5V+power+supply&amp;N=-1&amp;isNodeId=1</t>
+  </si>
+  <si>
+    <t>SEARCH RESULTS</t>
   </si>
 </sst>
 </file>
@@ -152,7 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,6 +190,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -186,6 +204,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -234,7 +255,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,7 +290,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -478,15 +499,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="28" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" style="4" customWidth="1"/>
@@ -582,11 +603,22 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>32</v>
+      </c>
       <c r="E5" s="4">
         <f>D5*C5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -667,7 +699,7 @@
       </c>
       <c r="E10" s="4">
         <f>SUM(E2:E9)</f>
-        <v>4336.08</v>
+        <v>4368.08</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,15 +718,30 @@
       <c r="C12" s="2">
         <f>C8*5</f>
         <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1"/>
     <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="B16" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated parts list - with shorter ethernet cables & meanwell powersupply
</commit_message>
<xml_diff>
--- a/testbed/parts_list.xlsx
+++ b/testbed/parts_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>URL</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Total Cost:</t>
   </si>
   <si>
-    <t>http://www.amazon.com/Cable-Matters-5-Color-Snagless-Ethernet/dp/B00E5I7VJG/ref=sr_1_1?s=pc&amp;ie=UTF8&amp;qid=1422383476&amp;sr=1-1&amp;keywords=ethernet+cables</t>
-  </si>
-  <si>
     <t>Ethernet Cable (5-set)</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>10/100 Ethernet Adapter (w/ linux)</t>
   </si>
   <si>
-    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16812315001&amp;cm_re=usb_ethernet-_-12-315-001-_-Product</t>
-  </si>
-  <si>
     <t>min cables required</t>
   </si>
   <si>
@@ -81,19 +75,16 @@
     <t>NETGEAR 48-Port 10/100/1000Mbps</t>
   </si>
   <si>
-    <t>Power  Supply</t>
-  </si>
-  <si>
-    <t>http://www.newegg.com/Product/Product.aspx?Item=9SIA5H62KH2141&amp;cm_re=300W_5V_power_supply-_-0R7-001B-00027-_-Product</t>
-  </si>
-  <si>
-    <t>Power Supply Search</t>
-  </si>
-  <si>
-    <t>http://www.newegg.com/Product/ProductList.aspx?Submit=ENE&amp;DEPA=0&amp;Order=BESTMATCH&amp;Description=300W+5V+power+supply&amp;N=-1&amp;isNodeId=1</t>
-  </si>
-  <si>
-    <t>SEARCH RESULTS</t>
+    <t>http://www.amazon.com/Meanwell-RSP-320-5-Power-Supply-OlympianLED/dp/B00IWC2RLS/ref=sr_1_1?ie=UTF8&amp;qid=1423685983&amp;sr=8-1&amp;keywords=meanwell+5v+300w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meanwell Power  Supply (5V, 60A, 300W) </t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Cable-Matters-5-Color-Snagless-Ethernet/dp/B00E5I7UAG/ref=sr_1_4?ie=UTF8&amp;qid=1423686055&amp;sr=8-4&amp;keywords=3ft.+ethernet+cable</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=9SIA2XB12C5920&amp;cm_re=usb_ethernet-_-9SIA2XB12C5920-_-Product</t>
   </si>
 </sst>
 </file>
@@ -167,7 +158,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,9 +179,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -499,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2">
         <v>32</v>
@@ -554,7 +542,7 @@
         <v>1760</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -562,7 +550,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -575,7 +563,7 @@
         <v>1315</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -604,51 +592,62 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="4">
-        <v>32</v>
+        <v>59.99</v>
       </c>
       <c r="E5" s="4">
         <f>D5*C5</f>
-        <v>32</v>
+        <v>59.99</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4">
+        <v>14.95</v>
+      </c>
       <c r="E6" s="4">
-        <f t="shared" ref="E6:E9" si="1">D6*C6</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="7"/>
+        <f t="shared" ref="E6:E8" si="1">D6*C6</f>
+        <v>478.4</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
         <v>15</v>
       </c>
-      <c r="C7" s="2">
-        <v>32</v>
-      </c>
       <c r="D7" s="4">
-        <v>11.99</v>
+        <v>10.99</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
-        <v>383.68</v>
+        <v>164.85</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,92 +655,60 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>13</v>
+        <v>396</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>396</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="D9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>396</v>
-      </c>
       <c r="E9" s="4">
-        <f t="shared" si="1"/>
-        <v>396</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="D10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4">
-        <f>SUM(E2:E9)</f>
-        <v>4368.08</v>
+        <f>SUM(E2:E8)</f>
+        <v>4460.6399999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C2*2</f>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
-        <f>C2*2</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2">
-        <f>C8*5</f>
+        <f>C7*5</f>
         <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F7" r:id="rId2"/>
     <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="B16" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>